<commit_message>
Minor fix in TSP.
</commit_message>
<xml_diff>
--- a/log/basline/run_1.xlsx
+++ b/log/basline/run_1.xlsx
@@ -405,7 +405,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3893</v>
+        <v>3476</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -416,7 +416,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3893</v>
+        <v>3716</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -427,7 +427,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>3893</v>
+        <v>3945</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -438,7 +438,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>3893</v>
+        <v>3945</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -449,7 +449,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>3986</v>
+        <v>3945</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -460,7 +460,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>3986</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -471,7 +471,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>4162</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -482,7 +482,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>4171</v>
+        <v>4613</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -493,7 +493,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>4216</v>
+        <v>4613</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -504,7 +504,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>4249</v>
+        <v>4692</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -515,7 +515,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>4333</v>
+        <v>4893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>